<commit_message>
add test for multi option check
</commit_message>
<xml_diff>
--- a/tests/_data/result.xlsx
+++ b/tests/_data/result.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="28800" windowHeight="12315"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="28800" windowHeight="12315"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="89">
   <si>
     <t>Q1</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>?</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
@@ -687,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BW4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="BC4" sqref="BC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1439,7 +1442,7 @@
         <v>77</v>
       </c>
       <c r="V4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="W4" t="s">
         <v>77</v>
@@ -1538,7 +1541,7 @@
         <v>75</v>
       </c>
       <c r="BC4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="BD4" t="s">
         <v>78</v>

</xml_diff>